<commit_message>
updated line sensor graphs
included axes and title
</commit_message>
<xml_diff>
--- a/Line Sensor Data 11.1 meeting.xlsx
+++ b/Line Sensor Data 11.1 meeting.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsmit\Documents\Arduino\libraries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29B3E8F1-55B1-4F0C-AA8E-226053C8FDCD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D315286A-DB4C-467E-9F80-1A5BA434CE41}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15200" windowHeight="6880" activeTab="1" xr2:uid="{A3D2CF52-304F-4CF3-AB79-E423AB2577AB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15200" windowHeight="6880" activeTab="1" xr2:uid="{A3D2CF52-304F-4CF3-AB79-E423AB2577AB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="MultiColor" sheetId="1" r:id="rId1"/>
+    <sheet name="Gray Zumo Mat" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>black#1</t>
   </si>
@@ -85,6 +85,30 @@
   </si>
   <si>
     <t>Grey #3</t>
+  </si>
+  <si>
+    <t>0 -Left Sensor</t>
+  </si>
+  <si>
+    <t>1-Middle Sensor</t>
+  </si>
+  <si>
+    <t>2-Right Sensor</t>
+  </si>
+  <si>
+    <t>From November 1st Brandeis Robotics Club meeting, represents the line sensor readings from a zumo robot as it was passed over the middle, egde, and outer edge of the grayscale zumo ring.</t>
+  </si>
+  <si>
+    <t>From November 1st Brandeis Robotics Club meeting, represents the line sensor readings from a zumo robot as it was passed over the middle, egde, and outer edge of the color zumo ring.</t>
+  </si>
+  <si>
+    <t>0-Left Sensor</t>
+  </si>
+  <si>
+    <t>1-middle sensor</t>
+  </si>
+  <si>
+    <t>2-right sensor</t>
   </si>
 </sst>
 </file>
@@ -154,6 +178,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> Line</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Sensor Reading Color Zumo Mat</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -186,48 +240,37 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>MultiColor!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0-Left Sensor</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="25400">
               <a:noFill/>
-              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>MultiColor!$A$2:$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -259,10 +302,10 @@
                 </c:pt>
               </c:strCache>
             </c:strRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$10</c:f>
+              <c:f>MultiColor!$B$2:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -295,8 +338,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
+          </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0C3A-4885-9FB8-1EC80E65C9E0}"/>
@@ -308,40 +350,28 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>MultiColor!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1-middle sensor</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln w="25400">
               <a:noFill/>
-              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>MultiColor!$A$2:$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -373,10 +403,10 @@
                 </c:pt>
               </c:strCache>
             </c:strRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$10</c:f>
+              <c:f>MultiColor!$C$2:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -409,8 +439,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
+          </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0C3A-4885-9FB8-1EC80E65C9E0}"/>
@@ -422,40 +451,28 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>MultiColor!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>2-right sensor</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln w="25400">
               <a:noFill/>
-              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>MultiColor!$A$2:$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -487,10 +504,10 @@
                 </c:pt>
               </c:strCache>
             </c:strRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$10</c:f>
+              <c:f>MultiColor!$D$2:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -523,8 +540,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
+          </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-0C3A-4885-9FB8-1EC80E65C9E0}"/>
@@ -539,10 +555,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:axId val="459125576"/>
         <c:axId val="459124264"/>
-      </c:scatterChart>
-      <c:valAx>
+      </c:barChart>
+      <c:catAx>
         <c:axId val="459125576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -588,8 +605,11 @@
         </c:txPr>
         <c:crossAx val="459124264"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="459124264"/>
         <c:scaling>
@@ -644,7 +664,7 @@
         </c:txPr>
         <c:crossAx val="459125576"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -744,6 +764,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Light</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Sensor Boundaries on grascale Zumo Mat</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -776,48 +826,37 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$B$1</c:f>
+              <c:f>'Gray Zumo Mat'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0 -Left Sensor</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="25400">
               <a:noFill/>
-              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$A$2:$A$10</c:f>
+              <c:f>'Gray Zumo Mat'!$A$2:$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -849,10 +888,10 @@
                 </c:pt>
               </c:strCache>
             </c:strRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$2:$B$10</c:f>
+              <c:f>'Gray Zumo Mat'!$B$2:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -885,8 +924,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
+          </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-05F0-4A90-945D-638E1B2E056D}"/>
@@ -898,40 +936,28 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$C$1</c:f>
+              <c:f>'Gray Zumo Mat'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1-Middle Sensor</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln w="25400">
               <a:noFill/>
-              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$A$2:$A$10</c:f>
+              <c:f>'Gray Zumo Mat'!$A$2:$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -963,10 +989,10 @@
                 </c:pt>
               </c:strCache>
             </c:strRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet2!$C$2:$C$10</c:f>
+              <c:f>'Gray Zumo Mat'!$C$2:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -999,8 +1025,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
+          </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-05F0-4A90-945D-638E1B2E056D}"/>
@@ -1012,40 +1037,28 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$D$1</c:f>
+              <c:f>'Gray Zumo Mat'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>2-Right Sensor</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln w="25400">
               <a:noFill/>
-              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$A$2:$A$10</c:f>
+              <c:f>'Gray Zumo Mat'!$A$2:$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -1077,10 +1090,10 @@
                 </c:pt>
               </c:strCache>
             </c:strRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet2!$D$2:$D$10</c:f>
+              <c:f>'Gray Zumo Mat'!$D$2:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1113,8 +1126,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
+          </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-05F0-4A90-945D-638E1B2E056D}"/>
@@ -1129,10 +1141,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:axId val="455544416"/>
         <c:axId val="455542448"/>
-      </c:scatterChart>
-      <c:valAx>
+      </c:barChart>
+      <c:catAx>
         <c:axId val="455544416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -1178,8 +1191,12 @@
         </c:txPr>
         <c:crossAx val="455542448"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickMarkSkip val="1"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="455542448"/>
         <c:scaling>
@@ -1234,7 +1251,7 @@
         </c:txPr>
         <c:crossAx val="455544416"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1244,6 +1261,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -2445,16 +2493,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>434975</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>130175</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2779,26 +2827,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2637A76B-1D30-40D7-9A8C-ADDC6BF4D156}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G19" sqref="C19:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.26953125" customWidth="1"/>
+    <col min="3" max="3" width="17.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>2</v>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -2925,6 +2974,11 @@
       </c>
       <c r="D10">
         <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -2935,23 +2989,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2235C11-3FDE-43E3-9EA4-1629BD4D6900}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="18.1796875" customWidth="1"/>
+    <col min="3" max="3" width="16.1796875" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>2</v>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -3078,6 +3137,11 @@
       </c>
       <c r="D10">
         <v>456</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added lprint line region exmaple file
allows robot to view all pats of the sumo ring and calculate thresholds
</commit_message>
<xml_diff>
--- a/Line Sensor Data 11.1 meeting.xlsx
+++ b/Line Sensor Data 11.1 meeting.xlsx
@@ -1,23 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsmit\Documents\Arduino\libraries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RTI\Documents\Arduino\libraries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC58D61-3E1F-4E95-9E7F-C16CF634F9D7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15200" windowHeight="6880" activeTab="2" xr2:uid="{A3D2CF52-304F-4CF3-AB79-E423AB2577AB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15195" windowHeight="6885" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MultiColor" sheetId="1" r:id="rId1"/>
     <sheet name="Gray Zumo Mat" sheetId="2" r:id="rId2"/>
-    <sheet name="Gray Zumo Mat Shield" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>black#1</t>
   </si>
@@ -111,17 +109,11 @@
   <si>
     <t>2-right sensor</t>
   </si>
-  <si>
-    <t>From January 17 Brandeis Robotics Club meeting, represents the line sensor readings from a zumo robot as it was passed over the middle, egde, and outer edge of the grayscale zumo ring.</t>
-  </si>
-  <si>
-    <t>For Zumo Shield robot</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -171,7 +163,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -346,7 +338,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0C3A-4885-9FB8-1EC80E65C9E0}"/>
             </c:ext>
@@ -447,7 +439,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0C3A-4885-9FB8-1EC80E65C9E0}"/>
             </c:ext>
@@ -548,7 +540,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-0C3A-4885-9FB8-1EC80E65C9E0}"/>
             </c:ext>
@@ -563,11 +555,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="459125576"/>
-        <c:axId val="459124264"/>
+        <c:axId val="389647384"/>
+        <c:axId val="389644248"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="459125576"/>
+        <c:axId val="389647384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -610,7 +602,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="459124264"/>
+        <c:crossAx val="389644248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -618,7 +610,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="459124264"/>
+        <c:axId val="389644248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -669,7 +661,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="459125576"/>
+        <c:crossAx val="389647384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -714,14 +706,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -757,7 +749,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -801,6 +793,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -932,7 +925,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-05F0-4A90-945D-638E1B2E056D}"/>
             </c:ext>
@@ -1033,7 +1026,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-05F0-4A90-945D-638E1B2E056D}"/>
             </c:ext>
@@ -1134,7 +1127,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-05F0-4A90-945D-638E1B2E056D}"/>
             </c:ext>
@@ -1149,11 +1142,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="455544416"/>
-        <c:axId val="455542448"/>
+        <c:axId val="389643072"/>
+        <c:axId val="389643464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="455544416"/>
+        <c:axId val="389643072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1196,7 +1189,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455542448"/>
+        <c:crossAx val="389643464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1205,7 +1198,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="455542448"/>
+        <c:axId val="389643464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1256,7 +1249,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455544416"/>
+        <c:crossAx val="389643072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1270,6 +1263,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1301,601 +1295,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Light</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Sensor Boundaries on grascale Zumo Mat</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Gray Zumo Mat Shield'!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0 -Left Sensor</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Gray Zumo Mat Shield'!$A$2:$A$10</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>Black#1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Black#2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Black#3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>White #1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>White #2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>White #3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Gray #1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Grey #2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Grey #3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Gray Zumo Mat Shield'!$B$2:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1332</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1328</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1328</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>148</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>164</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>140</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>712</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>716</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>748</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-789D-4A02-8FD1-8E993E7646B9}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Gray Zumo Mat Shield'!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1-Middle Sensor</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Gray Zumo Mat Shield'!$A$2:$A$10</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>Black#1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Black#2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Black#3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>White #1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>White #2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>White #3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Gray #1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Grey #2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Grey #3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Gray Zumo Mat Shield'!$C$2:$C$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>956</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>936</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>972</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>84</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>412</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>412</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>472</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-789D-4A02-8FD1-8E993E7646B9}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Gray Zumo Mat Shield'!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2-Right Sensor</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Gray Zumo Mat Shield'!$A$2:$A$10</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>Black#1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Black#2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Black#3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>White #1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>White #2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>White #3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Gray #1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Grey #2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Grey #3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Gray Zumo Mat Shield'!$D$2:$D$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1100</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1128</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1088</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>84</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>432</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>452</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>456</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-789D-4A02-8FD1-8E993E7646B9}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="455544416"/>
-        <c:axId val="455542448"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="455544416"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="455542448"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:tickMarkSkip val="1"/>
-        <c:noMultiLvlLbl val="1"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="455542448"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="455544416"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2010,46 +1417,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2567,522 +1934,6 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3618,7 +2469,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFFE29E8-ED01-4E1D-B988-C69FB9595F56}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EFFE29E8-ED01-4E1D-B988-C69FB9595F56}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3659,54 +2510,11 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8C9B45C-192D-4620-B66B-FC0EB343CFE1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A8C9B45C-192D-4620-B66B-FC0EB343CFE1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81CDBF10-E99E-4BBA-8655-4E45CED9F171}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -4019,20 +2827,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2637A76B-1D30-40D7-9A8C-ADDC6BF4D156}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="G19" sqref="C19:G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.26953125" customWidth="1"/>
-    <col min="3" max="3" width="17.08984375" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>23</v>
       </c>
@@ -4043,7 +2851,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4057,7 +2865,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -4071,7 +2879,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -4085,7 +2893,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -4099,7 +2907,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -4113,7 +2921,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -4127,7 +2935,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -4141,7 +2949,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -4155,7 +2963,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -4169,7 +2977,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -4181,21 +2989,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2235C11-3FDE-43E3-9EA4-1629BD4D6900}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B20" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.1796875" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>18</v>
       </c>
@@ -4206,7 +3014,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -4220,7 +3028,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -4234,7 +3042,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -4248,7 +3056,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -4262,7 +3070,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -4276,7 +3084,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -4290,7 +3098,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -4304,7 +3112,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -4318,7 +3126,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -4332,177 +3140,9 @@
         <v>456</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0EF6DC2-EF8E-41B9-B81F-D6F2FB6A874D}">
-  <dimension ref="A1:D22"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="18.1796875" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2">
-        <v>1332</v>
-      </c>
-      <c r="C2">
-        <v>956</v>
-      </c>
-      <c r="D2">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3">
-        <v>1328</v>
-      </c>
-      <c r="C3">
-        <v>936</v>
-      </c>
-      <c r="D3">
-        <v>1128</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>1328</v>
-      </c>
-      <c r="C4">
-        <v>972</v>
-      </c>
-      <c r="D4">
-        <v>1088</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5">
-        <v>148</v>
-      </c>
-      <c r="C5">
-        <v>68</v>
-      </c>
-      <c r="D5">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6">
-        <v>164</v>
-      </c>
-      <c r="C6">
-        <v>84</v>
-      </c>
-      <c r="D6">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7">
-        <v>140</v>
-      </c>
-      <c r="C7">
-        <v>60</v>
-      </c>
-      <c r="D7">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8">
-        <v>712</v>
-      </c>
-      <c r="C8">
-        <v>412</v>
-      </c>
-      <c r="D8">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9">
-        <v>716</v>
-      </c>
-      <c r="C9">
-        <v>412</v>
-      </c>
-      <c r="D9">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10">
-        <v>748</v>
-      </c>
-      <c r="C10">
-        <v>472</v>
-      </c>
-      <c r="D10">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>